<commit_message>
author : story ID : task :  Task breakdown Files added :  DeepakKumar.xlsx Files modified : DeepakKumar.xlsx Files deleted :  DeepakKumar.xlsx Description :  Replaced the original file after finning hours burnt
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/DeepakKumar.xlsx
+++ b/TeamDetails/TasksBreakDown/DeepakKumar.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7680" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7680" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Name 1" sheetId="1" r:id="rId1"/>
@@ -57,13 +57,7 @@
     <t>T50-1</t>
   </si>
   <si>
-    <t>Understanding of bigger picture</t>
-  </si>
-  <si>
     <t>T50-2</t>
-  </si>
-  <si>
-    <t>Understanding 'our' and 'their' database schema</t>
   </si>
   <si>
     <t>T50-3</t>
@@ -72,25 +66,31 @@
     <t>T50-4</t>
   </si>
   <si>
-    <t>Understanding their present excel sheets and drawing inferences</t>
-  </si>
-  <si>
-    <t>Creating MySql queries</t>
-  </si>
-  <si>
     <t>T50-5</t>
-  </si>
-  <si>
-    <t>Creating dummy DB for testing</t>
   </si>
   <si>
     <t>T50-6</t>
   </si>
   <si>
-    <t>Testing created queries in DB</t>
+    <t>Buffer Time</t>
   </si>
   <si>
-    <t>Buffer Time</t>
+    <t>Understand 'our' and 'their' database schema</t>
+  </si>
+  <si>
+    <t>Understand bigger picture</t>
+  </si>
+  <si>
+    <t>Understand current excel sheets and drawing inferences</t>
+  </si>
+  <si>
+    <t>Create MySql queries</t>
+  </si>
+  <si>
+    <t>Create dummy tables for testing</t>
+  </si>
+  <si>
+    <t>Test created queries in created tables</t>
   </si>
 </sst>
 </file>
@@ -2811,7 +2811,7 @@
   <dimension ref="A2:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2848,7 +2848,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="8">
@@ -2859,79 +2859,87 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
       <c r="G3" s="2">
         <f>E3-F3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
       <c r="G4" s="2">
         <f t="shared" ref="G4:G46" si="0">E4-F4</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2">
         <v>6</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2">
         <v>4</v>
@@ -2943,13 +2951,13 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
@@ -2961,11 +2969,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
@@ -3421,8 +3429,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B3:B9"/>
+    <mergeCell ref="A3:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author  :   Deepak Kumar Singh task    :   Task Burnout Updates Files added : none Files modified :  DeepakKumar.xlsx Files deleted : none
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/DeepakKumar.xlsx
+++ b/TeamDetails/TasksBreakDown/DeepakKumar.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak singh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship_2017_Prep.git\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t>Story ID</t>
   </si>
@@ -91,6 +91,36 @@
   </si>
   <si>
     <t>Test created queries in created tables</t>
+  </si>
+  <si>
+    <t>Total Hours Burnt</t>
+  </si>
+  <si>
+    <t>Hours Remaining</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Saved 1 hour</t>
+  </si>
+  <si>
+    <t>Saved 4 hour to be used in Testing</t>
+  </si>
+  <si>
+    <t>Continuing</t>
+  </si>
+  <si>
+    <t>Used 6 hours on 5/7/2017</t>
+  </si>
+  <si>
+    <t>DateOfCompletion</t>
   </si>
 </sst>
 </file>
@@ -200,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -226,6 +256,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2808,10 +2845,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G46"/>
+  <dimension ref="A2:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2821,10 +2858,14 @@
     <col min="4" max="4" width="67.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2846,8 +2887,17 @@
       <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -2871,8 +2921,14 @@
         <f>E3-F3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="13">
+        <v>42920</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="2" t="s">
@@ -2891,8 +2947,12 @@
         <f t="shared" ref="G4:G46" si="0">E4-F4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="13"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="2" t="s">
@@ -2911,8 +2971,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="2" t="s">
@@ -2931,8 +2998,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="2" t="s">
@@ -2951,8 +3025,17 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="12">
+        <v>42862</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="2" t="s">
@@ -2970,7 +3053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="2"/>
@@ -2986,89 +3069,75 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="6"/>
       <c r="E10" s="7"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="2"/>
+      <c r="D11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2">
+        <v>12</v>
+      </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="2"/>
+      <c r="D12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="2">
+        <v>6</v>
+      </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="3"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -3077,10 +3146,7 @@
       <c r="D17" s="3"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
@@ -3089,10 +3155,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
@@ -3101,10 +3164,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -3113,10 +3173,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
@@ -3125,10 +3182,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -3137,10 +3191,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
@@ -3149,10 +3200,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
@@ -3161,10 +3209,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -3173,10 +3218,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
@@ -3185,10 +3227,7 @@
       <c r="D26" s="3"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
@@ -3197,10 +3236,7 @@
       <c r="D27" s="3"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
@@ -3209,10 +3245,7 @@
       <c r="D28" s="3"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
@@ -3221,10 +3254,7 @@
       <c r="D29" s="3"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
@@ -3233,10 +3263,7 @@
       <c r="D30" s="3"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
@@ -3245,10 +3272,7 @@
       <c r="D31" s="3"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
@@ -3257,10 +3281,7 @@
       <c r="D32" s="3"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
@@ -3269,10 +3290,7 @@
       <c r="D33" s="3"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
@@ -3281,10 +3299,7 @@
       <c r="D34" s="3"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
@@ -3293,10 +3308,7 @@
       <c r="D35" s="3"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
@@ -3305,10 +3317,7 @@
       <c r="D36" s="3"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
@@ -3317,10 +3326,7 @@
       <c r="D37" s="3"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
@@ -3329,10 +3335,7 @@
       <c r="D38" s="3"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
@@ -3341,10 +3344,7 @@
       <c r="D39" s="3"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G39" s="2"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
@@ -3353,10 +3353,7 @@
       <c r="D40" s="3"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
-      <c r="G40" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
@@ -3365,10 +3362,7 @@
       <c r="D41" s="3"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G41" s="2"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
@@ -3377,10 +3371,7 @@
       <c r="D42" s="3"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
@@ -3389,10 +3380,7 @@
       <c r="D43" s="3"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
@@ -3401,10 +3389,7 @@
       <c r="D44" s="3"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
-      <c r="G44" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G44" s="2"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
@@ -3413,10 +3398,7 @@
       <c r="D45" s="3"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
-      <c r="G45" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G45" s="2"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
@@ -3425,15 +3407,13 @@
       <c r="D46" s="3"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G46" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B3:B9"/>
     <mergeCell ref="A3:A9"/>
+    <mergeCell ref="J3:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Task Burnout Updates Author: Deepak Kumar Singh Files Edited: DeepakKumar.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/DeepakKumar.xlsx
+++ b/TeamDetails/TasksBreakDown/DeepakKumar.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
   <si>
     <t>Story ID</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>DateOfCompletion</t>
+  </si>
+  <si>
+    <t>More than 3 conclusive hours is burnt in making up database with Pushkar Shukla</t>
   </si>
 </sst>
 </file>
@@ -230,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -249,6 +252,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -258,12 +264,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2848,7 +2859,7 @@
   <dimension ref="A2:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2887,21 +2898,21 @@
       <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="9">
         <f>SUM(E3:E9)</f>
         <v>18</v>
       </c>
@@ -2924,13 +2935,13 @@
       <c r="H3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="12">
         <v>42920</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
@@ -2944,17 +2955,17 @@
         <v>2</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G46" si="0">E4-F4</f>
+        <f t="shared" ref="G4:G9" si="0">E4-F4</f>
         <v>0</v>
       </c>
       <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="13"/>
+      <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
@@ -2977,11 +2988,11 @@
       <c r="I5" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="13"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
@@ -3004,11 +3015,11 @@
       <c r="I6" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="13"/>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
@@ -3031,13 +3042,13 @@
       <c r="I7" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="15">
         <v>42862</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
@@ -3047,15 +3058,23 @@
       <c r="E8" s="2">
         <v>2</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2">
+        <v>8</v>
+      </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>-6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="14">
+        <v>42893</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
         <v>14</v>
@@ -3063,11 +3082,17 @@
       <c r="E9" s="2">
         <v>1</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -3085,7 +3110,7 @@
         <v>21</v>
       </c>
       <c r="E11" s="2">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -3098,7 +3123,7 @@
         <v>22</v>
       </c>
       <c r="E12" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -3112,11 +3137,13 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -3410,10 +3437,11 @@
       <c r="G46" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B3:B9"/>
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="J3:J6"/>
+    <mergeCell ref="J8:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Total hours burnt updates Author: Deepak Kumar Singh Files edited : DeepakKumar.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/DeepakKumar.xlsx
+++ b/TeamDetails/TasksBreakDown/DeepakKumar.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship_2017_Prep.git\trunk\TeamDetails\TasksBreakDown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSDMS-v1\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,6 +18,9 @@
     <sheet name="Name 4" sheetId="5" r:id="rId4"/>
     <sheet name="Name 5" sheetId="6" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="31">
   <si>
     <t>Story ID</t>
   </si>
@@ -121,9 +124,6 @@
   </si>
   <si>
     <t>DateOfCompletion</t>
-  </si>
-  <si>
-    <t>More than 3 conclusive hours is burnt in making up database with Pushkar Shukla</t>
   </si>
 </sst>
 </file>
@@ -255,6 +255,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -267,21 +270,46 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2858,8 +2886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2909,12 +2937,12 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="10">
         <f>SUM(E3:E9)</f>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
@@ -2935,13 +2963,13 @@
       <c r="H3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="13">
         <v>42920</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
@@ -2961,11 +2989,11 @@
       <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="12"/>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
@@ -2973,14 +3001,14 @@
         <v>17</v>
       </c>
       <c r="E5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" t="s">
         <v>24</v>
@@ -2988,11 +3016,11 @@
       <c r="I5" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="12"/>
+      <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
@@ -3003,11 +3031,11 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H6" t="s">
         <v>24</v>
@@ -3015,11 +3043,11 @@
       <c r="I6" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="12"/>
+      <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
@@ -3027,14 +3055,14 @@
         <v>19</v>
       </c>
       <c r="E7" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F7" s="2">
         <v>6</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>-2</v>
+        <f>E7-F7</f>
+        <v>0</v>
       </c>
       <c r="H7" t="s">
         <v>28</v>
@@ -3042,13 +3070,13 @@
       <c r="I7" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="9">
         <v>42862</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
@@ -3056,14 +3084,14 @@
         <v>20</v>
       </c>
       <c r="E8" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F8" s="2">
         <v>8</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="H8" t="s">
         <v>24</v>
@@ -3073,17 +3101,17 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
@@ -3092,7 +3120,7 @@
       <c r="H9" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="13"/>
+      <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -3109,10 +3137,11 @@
       <c r="D11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="2">
-        <v>21</v>
-      </c>
-      <c r="F11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2">
+        <f>SUM(F3:F9)</f>
+        <v>24</v>
+      </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3137,13 +3166,11 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="D14" s="3"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>

</xml_diff>